<commit_message>
updated results and final code
</commit_message>
<xml_diff>
--- a/model_results/model_results.xlsx
+++ b/model_results/model_results.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,25 +486,47 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2024-07-10</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" t="n">
         <v>0.908</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" t="n">
         <v>0.91</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" t="n">
         <v>0.906</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" t="n">
         <v>0.8160065280783371</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" t="n">
         <v>0.966769</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>2024-07-10_v1</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.9155</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.9379999999999999</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.893</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.8318426675174775</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.9703179999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>